<commit_message>
melhorias solicitadas e adequação de banco de acordo com DER
</commit_message>
<xml_diff>
--- a/src/main/resources/net/gnfe/excel/produtos.xlsx
+++ b/src/main/resources/net/gnfe/excel/produtos.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guial\IdeaProjects\gnfe\src\resources\net\gnfe\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guial\IdeaProjects\projeto-tcc\src\main\resources\net\gnfe\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23E89410-F19A-48E7-82BE-4639FC8718FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53BB7EAD-284C-4679-A52C-AE2C61E6EF48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
     <author>Guilherme Alves da Silva</author>
   </authors>
   <commentList>
-    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{A9C5EC1B-37CD-4083-9B1C-87DE6A2724AA}">
+    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{A9C5EC1B-37CD-4083-9B1C-87DE6A2724AA}">
       <text>
         <r>
           <rPr>
@@ -39,7 +39,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P1" authorId="0" shapeId="0" xr:uid="{5423ED79-F508-4A0B-BDB9-45959247E52E}">
+    <comment ref="O1" authorId="0" shapeId="0" xr:uid="{5423ED79-F508-4A0B-BDB9-45959247E52E}">
       <text>
         <r>
           <rPr>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>ID</t>
   </si>
@@ -82,9 +82,6 @@
   </si>
   <si>
     <t>CFOP</t>
-  </si>
-  <si>
-    <t>Fornecedor ID</t>
   </si>
   <si>
     <t>Unidade Medida</t>
@@ -463,10 +460,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S1"/>
+  <dimension ref="A1:R1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -478,25 +475,24 @@
     <col min="5" max="6" width="30.7109375" customWidth="1"/>
     <col min="7" max="7" width="20" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.42578125" customWidth="1"/>
-    <col min="9" max="9" width="25" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="25" customWidth="1"/>
-    <col min="11" max="11" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="31.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="26.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="36.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="30.7109375" customWidth="1"/>
-    <col min="19" max="19" width="34.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="24" bestFit="1" customWidth="1"/>
-    <col min="21" max="22" width="24" customWidth="1"/>
-    <col min="23" max="23" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="30.28515625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25" customWidth="1"/>
+    <col min="10" max="10" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="31.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="36.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="30.7109375" customWidth="1"/>
+    <col min="18" max="18" width="34.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="24" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="24" customWidth="1"/>
+    <col min="22" max="22" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="27.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -522,19 +518,19 @@
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>10</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>12</v>
@@ -550,9 +546,6 @@
       </c>
       <c r="R1" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>